<commit_message>
fixes some test issues
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.17.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.17.balsamic.xlsx
@@ -1595,9 +1595,6 @@
     <t>skin</t>
   </si>
   <si>
-    <t>UDF/Bait set</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Estimated tumour purity (%): </t>
     </r>
@@ -2011,6 +2008,9 @@
   </si>
   <si>
     <t>Other elution buffer</t>
+  </si>
+  <si>
+    <t>UDF/Capture kit</t>
   </si>
 </sst>
 </file>
@@ -2617,7 +2617,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="338">
+  <cellStyleXfs count="340">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2882,6 +2882,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3555,7 +3557,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="338">
+  <cellStyles count="340">
     <cellStyle name="Excel Built-in Normal" xfId="45"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3851,6 +3853,8 @@
     <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4523,27 +4527,27 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="15" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15">
@@ -4629,7 +4633,7 @@
     </row>
     <row r="39" spans="1:5" ht="24">
       <c r="A39" s="34" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C39" s="15"/>
       <c r="E39" s="15"/>
@@ -4677,7 +4681,7 @@
     </row>
     <row r="50" spans="1:1" ht="24">
       <c r="A50" s="34" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="51" spans="1:1">
@@ -4690,7 +4694,7 @@
     </row>
     <row r="53" spans="1:1" ht="36">
       <c r="A53" s="176" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:1">
@@ -4698,7 +4702,7 @@
     </row>
     <row r="55" spans="1:1" ht="24">
       <c r="A55" s="34" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="1:1">
@@ -4804,8 +4808,8 @@
   </sheetPr>
   <dimension ref="A1:AE428"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A63" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0"/>
@@ -5145,7 +5149,7 @@
       </c>
       <c r="AE9" s="205"/>
     </row>
-    <row r="10" spans="1:31" s="102" customFormat="1" ht="13" hidden="1" customHeight="1">
+    <row r="10" spans="1:31" s="102" customFormat="1" ht="13" customHeight="1">
       <c r="A10" s="103" t="s">
         <v>0</v>
       </c>
@@ -5180,7 +5184,7 @@
       <c r="AD10" s="104"/>
       <c r="AE10" s="104"/>
     </row>
-    <row r="11" spans="1:31" s="118" customFormat="1" ht="41" hidden="1" customHeight="1">
+    <row r="11" spans="1:31" s="118" customFormat="1" ht="41" customHeight="1">
       <c r="A11" s="106" t="s">
         <v>1</v>
       </c>
@@ -5236,11 +5240,11 @@
       </c>
       <c r="T11" s="114"/>
       <c r="U11" s="194" t="s">
-        <v>388</v>
+        <v>509</v>
       </c>
       <c r="V11" s="179"/>
       <c r="W11" s="195" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="X11" s="115" t="s">
         <v>278</v>
@@ -5263,7 +5267,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="126" customFormat="1" ht="19" hidden="1" customHeight="1">
+    <row r="12" spans="1:31" s="126" customFormat="1" ht="19" customHeight="1">
       <c r="A12" s="103" t="s">
         <v>5</v>
       </c>
@@ -5358,7 +5362,7 @@
       </c>
       <c r="V13" s="181"/>
       <c r="W13" s="140" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="X13" s="140" t="s">
         <v>296</v>
@@ -5418,7 +5422,7 @@
     </row>
     <row r="15" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A15" s="55" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B15" s="53" t="s">
         <v>37</v>
@@ -5427,10 +5431,10 @@
         <v>299</v>
       </c>
       <c r="D15" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="E15" s="55" t="s">
         <v>433</v>
-      </c>
-      <c r="E15" s="55" t="s">
-        <v>434</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>15</v>
@@ -5452,7 +5456,7 @@
       </c>
       <c r="L15" s="149"/>
       <c r="M15" s="58" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="N15" s="57" t="s">
         <v>27</v>
@@ -5465,12 +5469,12 @@
         <v>300</v>
       </c>
       <c r="R15" s="55" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S15" s="60"/>
       <c r="T15" s="150"/>
       <c r="U15" s="21" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="V15" s="180"/>
       <c r="W15" s="198"/>
@@ -5489,15 +5493,15 @@
       </c>
       <c r="AC15" s="152"/>
       <c r="AD15" s="58" t="s">
+        <v>501</v>
+      </c>
+      <c r="AE15" s="58" t="s">
         <v>502</v>
-      </c>
-      <c r="AE15" s="58" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="16" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A16" s="55" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B16" s="53" t="s">
         <v>37</v>
@@ -5509,7 +5513,7 @@
         <v>285</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F16" s="54" t="s">
         <v>16</v>
@@ -5543,7 +5547,7 @@
       <c r="S16" s="60"/>
       <c r="T16" s="150"/>
       <c r="U16" s="33" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="V16" s="180"/>
       <c r="W16" s="198"/>
@@ -5562,7 +5566,7 @@
     </row>
     <row r="17" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A17" s="55" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B17" s="53" t="s">
         <v>37</v>
@@ -5574,7 +5578,7 @@
         <v>286</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F17" s="54" t="s">
         <v>15</v>
@@ -5608,7 +5612,7 @@
       <c r="S17" s="60"/>
       <c r="T17" s="150"/>
       <c r="U17" s="21" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="V17" s="180"/>
       <c r="W17" s="198"/>
@@ -5625,7 +5629,7 @@
     </row>
     <row r="18" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A18" s="55" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B18" s="53" t="s">
         <v>37</v>
@@ -5637,7 +5641,7 @@
         <v>287</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F18" s="54" t="s">
         <v>77</v>
@@ -5671,7 +5675,7 @@
       <c r="S18" s="60"/>
       <c r="T18" s="150"/>
       <c r="U18" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V18" s="180"/>
       <c r="W18" s="61"/>
@@ -5688,7 +5692,7 @@
     </row>
     <row r="19" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="55" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B19" s="53" t="s">
         <v>37</v>
@@ -5700,7 +5704,7 @@
         <v>288</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F19" s="54" t="s">
         <v>77</v>
@@ -5734,7 +5738,7 @@
       <c r="S19" s="60"/>
       <c r="T19" s="150"/>
       <c r="U19" s="21" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="V19" s="180"/>
       <c r="W19" s="61"/>
@@ -5751,7 +5755,7 @@
     </row>
     <row r="20" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="55" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B20" s="53" t="s">
         <v>37</v>
@@ -5763,7 +5767,7 @@
         <v>289</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F20" s="54" t="s">
         <v>77</v>
@@ -5797,7 +5801,7 @@
       <c r="S20" s="60"/>
       <c r="T20" s="150"/>
       <c r="U20" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V20" s="180"/>
       <c r="W20" s="61"/>
@@ -5814,7 +5818,7 @@
     </row>
     <row r="21" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A21" s="55" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B21" s="53" t="s">
         <v>37</v>
@@ -5826,7 +5830,7 @@
         <v>290</v>
       </c>
       <c r="E21" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F21" s="54" t="s">
         <v>77</v>
@@ -5860,7 +5864,7 @@
       <c r="S21" s="60"/>
       <c r="T21" s="150"/>
       <c r="U21" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V21" s="180"/>
       <c r="W21" s="61"/>
@@ -5877,7 +5881,7 @@
     </row>
     <row r="22" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A22" s="55" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B22" s="53" t="s">
         <v>37</v>
@@ -5886,10 +5890,10 @@
         <v>299</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F22" s="54" t="s">
         <v>77</v>
@@ -5923,7 +5927,7 @@
       <c r="S22" s="60"/>
       <c r="T22" s="150"/>
       <c r="U22" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V22" s="180"/>
       <c r="W22" s="61"/>
@@ -5940,7 +5944,7 @@
     </row>
     <row r="23" spans="1:31" ht="25" customHeight="1">
       <c r="A23" s="55" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B23" s="53" t="s">
         <v>37</v>
@@ -5949,10 +5953,10 @@
         <v>299</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F23" s="54" t="s">
         <v>77</v>
@@ -5986,7 +5990,7 @@
       <c r="S23" s="60"/>
       <c r="T23" s="150"/>
       <c r="U23" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V23" s="180"/>
       <c r="W23" s="61"/>
@@ -6003,7 +6007,7 @@
     </row>
     <row r="24" spans="1:31" ht="25" customHeight="1">
       <c r="A24" s="55" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B24" s="53" t="s">
         <v>37</v>
@@ -6012,10 +6016,10 @@
         <v>299</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F24" s="54" t="s">
         <v>77</v>
@@ -6049,7 +6053,7 @@
       <c r="S24" s="60"/>
       <c r="T24" s="150"/>
       <c r="U24" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V24" s="180"/>
       <c r="W24" s="61"/>
@@ -6066,7 +6070,7 @@
     </row>
     <row r="25" spans="1:31" ht="25" customHeight="1">
       <c r="A25" s="55" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B25" s="53" t="s">
         <v>37</v>
@@ -6075,10 +6079,10 @@
         <v>299</v>
       </c>
       <c r="D25" s="29" t="s">
+        <v>447</v>
+      </c>
+      <c r="E25" s="55" t="s">
         <v>448</v>
-      </c>
-      <c r="E25" s="55" t="s">
-        <v>449</v>
       </c>
       <c r="F25" s="54" t="s">
         <v>77</v>
@@ -6112,11 +6116,11 @@
       <c r="S25" s="60"/>
       <c r="T25" s="150"/>
       <c r="U25" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V25" s="180"/>
       <c r="W25" s="61" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="X25" s="21">
         <v>55</v>
@@ -6128,12 +6132,12 @@
       <c r="AC25" s="152"/>
       <c r="AD25" s="58"/>
       <c r="AE25" s="58" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="26" spans="1:31" ht="25" customHeight="1">
       <c r="A26" s="55" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B26" s="53" t="s">
         <v>37</v>
@@ -6142,10 +6146,10 @@
         <v>299</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E26" s="55" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>77</v>
@@ -6179,11 +6183,11 @@
       <c r="S26" s="60"/>
       <c r="T26" s="150"/>
       <c r="U26" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V26" s="180"/>
       <c r="W26" s="61" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="X26" s="21">
         <v>60</v>
@@ -6198,7 +6202,7 @@
     </row>
     <row r="27" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="55" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B27" s="53" t="s">
         <v>37</v>
@@ -6207,10 +6211,10 @@
         <v>299</v>
       </c>
       <c r="D27" s="197" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E27" s="55" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F27" s="54" t="s">
         <v>77</v>
@@ -6244,11 +6248,11 @@
       <c r="S27" s="60"/>
       <c r="T27" s="150"/>
       <c r="U27" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V27" s="180"/>
       <c r="W27" s="61" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="X27" s="21">
         <v>65</v>
@@ -6263,7 +6267,7 @@
     </row>
     <row r="28" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="55" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B28" s="53" t="s">
         <v>37</v>
@@ -6272,10 +6276,10 @@
         <v>299</v>
       </c>
       <c r="D28" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="E28" s="55" t="s">
         <v>454</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>455</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>77</v>
@@ -6309,11 +6313,11 @@
       <c r="S28" s="60"/>
       <c r="T28" s="150"/>
       <c r="U28" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V28" s="180"/>
       <c r="W28" s="61" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="X28" s="21">
         <v>70</v>
@@ -6328,7 +6332,7 @@
     </row>
     <row r="29" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A29" s="55" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B29" s="53" t="s">
         <v>37</v>
@@ -6340,7 +6344,7 @@
         <v>249</v>
       </c>
       <c r="E29" s="55" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F29" s="54" t="s">
         <v>77</v>
@@ -6374,11 +6378,11 @@
       <c r="S29" s="60"/>
       <c r="T29" s="150"/>
       <c r="U29" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V29" s="180"/>
       <c r="W29" s="61" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="X29" s="21">
         <v>75</v>
@@ -6393,7 +6397,7 @@
     </row>
     <row r="30" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="55" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B30" s="53" t="s">
         <v>37</v>
@@ -6405,7 +6409,7 @@
         <v>364</v>
       </c>
       <c r="E30" s="55" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F30" s="54" t="s">
         <v>77</v>
@@ -6439,11 +6443,11 @@
       <c r="S30" s="60"/>
       <c r="T30" s="150"/>
       <c r="U30" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V30" s="180"/>
       <c r="W30" s="61" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="X30" s="21">
         <v>80</v>
@@ -6458,7 +6462,7 @@
     </row>
     <row r="31" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A31" s="55" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B31" s="53" t="s">
         <v>37</v>
@@ -6467,10 +6471,10 @@
         <v>299</v>
       </c>
       <c r="D31" s="29" t="s">
+        <v>458</v>
+      </c>
+      <c r="E31" s="55" t="s">
         <v>459</v>
-      </c>
-      <c r="E31" s="55" t="s">
-        <v>460</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>77</v>
@@ -6504,7 +6508,7 @@
       <c r="S31" s="60"/>
       <c r="T31" s="150"/>
       <c r="U31" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V31" s="180"/>
       <c r="W31" s="61"/>
@@ -6521,7 +6525,7 @@
     </row>
     <row r="32" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="55" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B32" s="53" t="s">
         <v>37</v>
@@ -6530,10 +6534,10 @@
         <v>299</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>77</v>
@@ -6567,7 +6571,7 @@
       <c r="S32" s="60"/>
       <c r="T32" s="150"/>
       <c r="U32" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V32" s="180"/>
       <c r="W32" s="61"/>
@@ -6584,7 +6588,7 @@
     </row>
     <row r="33" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A33" s="39" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B33" s="53" t="s">
         <v>37</v>
@@ -6596,7 +6600,7 @@
         <v>285</v>
       </c>
       <c r="E33" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>77</v>
@@ -6630,7 +6634,7 @@
       <c r="S33" s="60"/>
       <c r="T33" s="150"/>
       <c r="U33" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V33" s="180"/>
       <c r="W33" s="61"/>
@@ -6647,7 +6651,7 @@
     </row>
     <row r="34" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A34" s="39" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B34" s="53" t="s">
         <v>37</v>
@@ -6659,7 +6663,7 @@
         <v>285</v>
       </c>
       <c r="E34" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F34" s="54" t="s">
         <v>77</v>
@@ -6693,7 +6697,7 @@
       <c r="S34" s="60"/>
       <c r="T34" s="150"/>
       <c r="U34" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V34" s="180"/>
       <c r="W34" s="61"/>
@@ -6710,7 +6714,7 @@
     </row>
     <row r="35" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A35" s="39" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B35" s="53" t="s">
         <v>37</v>
@@ -6722,7 +6726,7 @@
         <v>285</v>
       </c>
       <c r="E35" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>77</v>
@@ -6756,7 +6760,7 @@
       <c r="S35" s="60"/>
       <c r="T35" s="150"/>
       <c r="U35" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V35" s="180"/>
       <c r="W35" s="61"/>
@@ -6773,7 +6777,7 @@
     </row>
     <row r="36" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A36" s="39" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B36" s="53" t="s">
         <v>37</v>
@@ -6785,7 +6789,7 @@
         <v>285</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>77</v>
@@ -6819,7 +6823,7 @@
       <c r="S36" s="60"/>
       <c r="T36" s="150"/>
       <c r="U36" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V36" s="180"/>
       <c r="W36" s="61"/>
@@ -6836,7 +6840,7 @@
     </row>
     <row r="37" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A37" s="39" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B37" s="53" t="s">
         <v>37</v>
@@ -6848,7 +6852,7 @@
         <v>285</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>77</v>
@@ -6882,7 +6886,7 @@
       <c r="S37" s="60"/>
       <c r="T37" s="150"/>
       <c r="U37" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V37" s="180"/>
       <c r="W37" s="61"/>
@@ -6899,7 +6903,7 @@
     </row>
     <row r="38" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
       <c r="A38" s="39" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B38" s="53" t="s">
         <v>37</v>
@@ -6911,7 +6915,7 @@
         <v>285</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>77</v>
@@ -6945,7 +6949,7 @@
       <c r="S38" s="60"/>
       <c r="T38" s="150"/>
       <c r="U38" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V38" s="180"/>
       <c r="W38" s="61"/>
@@ -6962,7 +6966,7 @@
     </row>
     <row r="39" spans="1:31" ht="25" customHeight="1">
       <c r="A39" s="39" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B39" s="53" t="s">
         <v>37</v>
@@ -6974,7 +6978,7 @@
         <v>285</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>77</v>
@@ -7008,7 +7012,7 @@
       <c r="S39" s="60"/>
       <c r="T39" s="150"/>
       <c r="U39" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V39" s="180"/>
       <c r="W39" s="61"/>
@@ -7025,7 +7029,7 @@
     </row>
     <row r="40" spans="1:31" ht="25" customHeight="1">
       <c r="A40" s="39" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B40" s="53" t="s">
         <v>37</v>
@@ -7037,7 +7041,7 @@
         <v>285</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>77</v>
@@ -7071,7 +7075,7 @@
       <c r="S40" s="60"/>
       <c r="T40" s="150"/>
       <c r="U40" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V40" s="180"/>
       <c r="W40" s="61"/>
@@ -7088,7 +7092,7 @@
     </row>
     <row r="41" spans="1:31" ht="25" customHeight="1">
       <c r="A41" s="39" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B41" s="53" t="s">
         <v>37</v>
@@ -7100,7 +7104,7 @@
         <v>285</v>
       </c>
       <c r="E41" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>77</v>
@@ -7134,7 +7138,7 @@
       <c r="S41" s="60"/>
       <c r="T41" s="150"/>
       <c r="U41" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V41" s="180"/>
       <c r="W41" s="61"/>
@@ -7151,7 +7155,7 @@
     </row>
     <row r="42" spans="1:31" ht="25" customHeight="1">
       <c r="A42" s="39" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B42" s="53" t="s">
         <v>37</v>
@@ -7163,7 +7167,7 @@
         <v>285</v>
       </c>
       <c r="E42" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>77</v>
@@ -7197,7 +7201,7 @@
       <c r="S42" s="60"/>
       <c r="T42" s="150"/>
       <c r="U42" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V42" s="180"/>
       <c r="W42" s="61"/>
@@ -7214,7 +7218,7 @@
     </row>
     <row r="43" spans="1:31" ht="25" customHeight="1">
       <c r="A43" s="39" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B43" s="53" t="s">
         <v>37</v>
@@ -7226,7 +7230,7 @@
         <v>285</v>
       </c>
       <c r="E43" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>77</v>
@@ -7260,7 +7264,7 @@
       <c r="S43" s="60"/>
       <c r="T43" s="150"/>
       <c r="U43" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V43" s="180"/>
       <c r="W43" s="61"/>
@@ -7277,7 +7281,7 @@
     </row>
     <row r="44" spans="1:31" ht="25" customHeight="1">
       <c r="A44" s="39" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B44" s="53" t="s">
         <v>37</v>
@@ -7289,7 +7293,7 @@
         <v>285</v>
       </c>
       <c r="E44" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>77</v>
@@ -7323,7 +7327,7 @@
       <c r="S44" s="60"/>
       <c r="T44" s="150"/>
       <c r="U44" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V44" s="180"/>
       <c r="W44" s="61"/>
@@ -7340,7 +7344,7 @@
     </row>
     <row r="45" spans="1:31" ht="25" customHeight="1">
       <c r="A45" s="39" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B45" s="53" t="s">
         <v>37</v>
@@ -7352,7 +7356,7 @@
         <v>285</v>
       </c>
       <c r="E45" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>77</v>
@@ -7386,7 +7390,7 @@
       <c r="S45" s="60"/>
       <c r="T45" s="150"/>
       <c r="U45" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V45" s="180"/>
       <c r="W45" s="61"/>
@@ -7403,7 +7407,7 @@
     </row>
     <row r="46" spans="1:31" ht="25" customHeight="1">
       <c r="A46" s="39" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B46" s="53" t="s">
         <v>37</v>
@@ -7415,7 +7419,7 @@
         <v>285</v>
       </c>
       <c r="E46" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>77</v>
@@ -7449,7 +7453,7 @@
       <c r="S46" s="60"/>
       <c r="T46" s="150"/>
       <c r="U46" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V46" s="180"/>
       <c r="W46" s="61"/>
@@ -7466,7 +7470,7 @@
     </row>
     <row r="47" spans="1:31" ht="25" customHeight="1">
       <c r="A47" s="39" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B47" s="53" t="s">
         <v>37</v>
@@ -7478,7 +7482,7 @@
         <v>285</v>
       </c>
       <c r="E47" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>77</v>
@@ -7512,7 +7516,7 @@
       <c r="S47" s="60"/>
       <c r="T47" s="150"/>
       <c r="U47" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V47" s="180"/>
       <c r="W47" s="61"/>
@@ -7529,7 +7533,7 @@
     </row>
     <row r="48" spans="1:31" ht="25" customHeight="1">
       <c r="A48" s="39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B48" s="53" t="s">
         <v>37</v>
@@ -7541,7 +7545,7 @@
         <v>285</v>
       </c>
       <c r="E48" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>77</v>
@@ -7575,7 +7579,7 @@
       <c r="S48" s="60"/>
       <c r="T48" s="150"/>
       <c r="U48" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V48" s="180"/>
       <c r="W48" s="61"/>
@@ -7592,7 +7596,7 @@
     </row>
     <row r="49" spans="1:31" ht="25" customHeight="1">
       <c r="A49" s="39" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>37</v>
@@ -7604,7 +7608,7 @@
         <v>285</v>
       </c>
       <c r="E49" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>77</v>
@@ -7638,7 +7642,7 @@
       <c r="S49" s="60"/>
       <c r="T49" s="150"/>
       <c r="U49" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V49" s="180"/>
       <c r="W49" s="61"/>
@@ -7655,7 +7659,7 @@
     </row>
     <row r="50" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="39" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B50" s="53" t="s">
         <v>37</v>
@@ -7667,7 +7671,7 @@
         <v>285</v>
       </c>
       <c r="E50" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>77</v>
@@ -7701,7 +7705,7 @@
       <c r="S50" s="60"/>
       <c r="T50" s="150"/>
       <c r="U50" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V50" s="180"/>
       <c r="W50" s="61"/>
@@ -7718,7 +7722,7 @@
     </row>
     <row r="51" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A51" s="39" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B51" s="53" t="s">
         <v>37</v>
@@ -7730,7 +7734,7 @@
         <v>285</v>
       </c>
       <c r="E51" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>77</v>
@@ -7764,7 +7768,7 @@
       <c r="S51" s="60"/>
       <c r="T51" s="150"/>
       <c r="U51" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V51" s="180"/>
       <c r="W51" s="61"/>
@@ -7781,7 +7785,7 @@
     </row>
     <row r="52" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A52" s="39" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B52" s="53" t="s">
         <v>37</v>
@@ -7793,7 +7797,7 @@
         <v>285</v>
       </c>
       <c r="E52" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>77</v>
@@ -7827,7 +7831,7 @@
       <c r="S52" s="60"/>
       <c r="T52" s="150"/>
       <c r="U52" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V52" s="180"/>
       <c r="W52" s="61"/>
@@ -7844,7 +7848,7 @@
     </row>
     <row r="53" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A53" s="39" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B53" s="53" t="s">
         <v>37</v>
@@ -7856,7 +7860,7 @@
         <v>285</v>
       </c>
       <c r="E53" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>77</v>
@@ -7890,7 +7894,7 @@
       <c r="S53" s="60"/>
       <c r="T53" s="150"/>
       <c r="U53" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V53" s="180"/>
       <c r="W53" s="61"/>
@@ -7907,7 +7911,7 @@
     </row>
     <row r="54" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A54" s="39" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B54" s="53" t="s">
         <v>37</v>
@@ -7919,7 +7923,7 @@
         <v>285</v>
       </c>
       <c r="E54" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>77</v>
@@ -7953,7 +7957,7 @@
       <c r="S54" s="60"/>
       <c r="T54" s="150"/>
       <c r="U54" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V54" s="180"/>
       <c r="W54" s="61"/>
@@ -7970,7 +7974,7 @@
     </row>
     <row r="55" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A55" s="39" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B55" s="53" t="s">
         <v>37</v>
@@ -7982,7 +7986,7 @@
         <v>285</v>
       </c>
       <c r="E55" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>77</v>
@@ -8016,7 +8020,7 @@
       <c r="S55" s="60"/>
       <c r="T55" s="150"/>
       <c r="U55" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V55" s="180"/>
       <c r="W55" s="61"/>
@@ -8033,7 +8037,7 @@
     </row>
     <row r="56" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A56" s="39" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B56" s="53" t="s">
         <v>37</v>
@@ -8045,7 +8049,7 @@
         <v>285</v>
       </c>
       <c r="E56" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>77</v>
@@ -8079,7 +8083,7 @@
       <c r="S56" s="60"/>
       <c r="T56" s="150"/>
       <c r="U56" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V56" s="180"/>
       <c r="W56" s="61"/>
@@ -8096,7 +8100,7 @@
     </row>
     <row r="57" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A57" s="39" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B57" s="53" t="s">
         <v>37</v>
@@ -8108,7 +8112,7 @@
         <v>285</v>
       </c>
       <c r="E57" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>77</v>
@@ -8142,7 +8146,7 @@
       <c r="S57" s="60"/>
       <c r="T57" s="150"/>
       <c r="U57" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V57" s="180"/>
       <c r="W57" s="61"/>
@@ -8159,7 +8163,7 @@
     </row>
     <row r="58" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A58" s="39" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B58" s="53" t="s">
         <v>37</v>
@@ -8171,7 +8175,7 @@
         <v>285</v>
       </c>
       <c r="E58" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>77</v>
@@ -8205,7 +8209,7 @@
       <c r="S58" s="60"/>
       <c r="T58" s="150"/>
       <c r="U58" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V58" s="180"/>
       <c r="W58" s="61"/>
@@ -8222,7 +8226,7 @@
     </row>
     <row r="59" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A59" s="39" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B59" s="53" t="s">
         <v>37</v>
@@ -8234,7 +8238,7 @@
         <v>285</v>
       </c>
       <c r="E59" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F59" s="54" t="s">
         <v>77</v>
@@ -8268,7 +8272,7 @@
       <c r="S59" s="60"/>
       <c r="T59" s="150"/>
       <c r="U59" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V59" s="180"/>
       <c r="W59" s="61"/>
@@ -8285,7 +8289,7 @@
     </row>
     <row r="60" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A60" s="39" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B60" s="53" t="s">
         <v>37</v>
@@ -8297,7 +8301,7 @@
         <v>285</v>
       </c>
       <c r="E60" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F60" s="54" t="s">
         <v>77</v>
@@ -8322,7 +8326,7 @@
       <c r="N60" s="57"/>
       <c r="O60" s="149"/>
       <c r="P60" s="30" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q60" s="56" t="s">
         <v>77</v>
@@ -8331,7 +8335,7 @@
       <c r="S60" s="60"/>
       <c r="T60" s="150"/>
       <c r="U60" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V60" s="180"/>
       <c r="W60" s="61"/>
@@ -8348,7 +8352,7 @@
     </row>
     <row r="61" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A61" s="39" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B61" s="53" t="s">
         <v>37</v>
@@ -8360,7 +8364,7 @@
         <v>285</v>
       </c>
       <c r="E61" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>77</v>
@@ -8394,7 +8398,7 @@
       <c r="S61" s="60"/>
       <c r="T61" s="150"/>
       <c r="U61" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V61" s="180"/>
       <c r="W61" s="61"/>
@@ -8411,7 +8415,7 @@
     </row>
     <row r="62" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A62" s="39" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B62" s="53" t="s">
         <v>37</v>
@@ -8423,7 +8427,7 @@
         <v>285</v>
       </c>
       <c r="E62" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F62" s="54" t="s">
         <v>77</v>
@@ -8457,7 +8461,7 @@
       <c r="S62" s="60"/>
       <c r="T62" s="150"/>
       <c r="U62" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V62" s="180"/>
       <c r="W62" s="61"/>
@@ -8474,7 +8478,7 @@
     </row>
     <row r="63" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
       <c r="A63" s="39" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B63" s="53" t="s">
         <v>37</v>
@@ -8486,7 +8490,7 @@
         <v>285</v>
       </c>
       <c r="E63" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F63" s="54" t="s">
         <v>77</v>
@@ -8511,7 +8515,7 @@
       <c r="N63" s="57"/>
       <c r="O63" s="149"/>
       <c r="P63" s="166" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q63" s="56" t="s">
         <v>77</v>
@@ -8520,7 +8524,7 @@
       <c r="S63" s="60"/>
       <c r="T63" s="150"/>
       <c r="U63" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V63" s="180"/>
       <c r="W63" s="61"/>
@@ -8537,7 +8541,7 @@
     </row>
     <row r="64" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
       <c r="A64" s="39" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B64" s="53" t="s">
         <v>37</v>
@@ -8549,7 +8553,7 @@
         <v>285</v>
       </c>
       <c r="E64" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F64" s="54" t="s">
         <v>77</v>
@@ -8574,7 +8578,7 @@
       <c r="N64" s="57"/>
       <c r="O64" s="149"/>
       <c r="P64" s="166" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Q64" s="56" t="s">
         <v>77</v>
@@ -8583,7 +8587,7 @@
       <c r="S64" s="60"/>
       <c r="T64" s="150"/>
       <c r="U64" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V64" s="180"/>
       <c r="W64" s="61"/>
@@ -8600,7 +8604,7 @@
     </row>
     <row r="65" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
       <c r="A65" s="39" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B65" s="53" t="s">
         <v>37</v>
@@ -8612,7 +8616,7 @@
         <v>285</v>
       </c>
       <c r="E65" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F65" s="54" t="s">
         <v>77</v>
@@ -8646,7 +8650,7 @@
       <c r="S65" s="60"/>
       <c r="T65" s="150"/>
       <c r="U65" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V65" s="180"/>
       <c r="W65" s="61"/>
@@ -8663,7 +8667,7 @@
     </row>
     <row r="66" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
       <c r="A66" s="39" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B66" s="53" t="s">
         <v>37</v>
@@ -8675,7 +8679,7 @@
         <v>285</v>
       </c>
       <c r="E66" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F66" s="54" t="s">
         <v>77</v>
@@ -8709,7 +8713,7 @@
       <c r="S66" s="60"/>
       <c r="T66" s="150"/>
       <c r="U66" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V66" s="180"/>
       <c r="W66" s="61"/>
@@ -19749,7 +19753,7 @@
       <c r="AB428" s="163"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tGOhRZ2XwULkBx8gD7BqKRbDdzQFPxygT+aCC0tienHUrn+HF12C7woGUWPW9hLnO2rzKmr+GbEyL9CvlL7egw==" saltValue="f4JcKEPHxAcUDSAHw0bpng==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="W9:X9"/>
     <mergeCell ref="A9:K9"/>
@@ -19953,7 +19957,7 @@
         <v>284</v>
       </c>
       <c r="K2" s="26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L2" s="27" t="s">
         <v>80</v>
@@ -19999,7 +20003,7 @@
         <v>355</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>15</v>
@@ -20023,7 +20027,7 @@
         <v>300</v>
       </c>
       <c r="K3" s="173" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="L3" s="167" t="s">
         <v>27</v>
@@ -20077,7 +20081,7 @@
         <v>301</v>
       </c>
       <c r="K4" s="173" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="L4" s="168" t="s">
         <v>28</v>
@@ -20125,7 +20129,7 @@
         <v>77</v>
       </c>
       <c r="K5" s="173" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L5" s="168" t="s">
         <v>29</v>
@@ -20293,7 +20297,7 @@
       <c r="A10" s="31"/>
       <c r="B10" s="7"/>
       <c r="C10" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="20" t="s">
@@ -20328,7 +20332,7 @@
     <row r="11" spans="1:38">
       <c r="A11" s="31"/>
       <c r="C11" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="20" t="s">
@@ -20364,7 +20368,7 @@
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
       <c r="C12" s="29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="20" t="s">
@@ -20400,7 +20404,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="32"/>
       <c r="C13" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="20" t="s">
@@ -20436,7 +20440,7 @@
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D14" s="21"/>
       <c r="E14" s="20" t="s">
@@ -20472,7 +20476,7 @@
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="20" t="s">
@@ -20541,7 +20545,7 @@
       <c r="A17" s="31"/>
       <c r="B17" s="33"/>
       <c r="C17" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D17" s="21"/>
       <c r="E17" s="20" t="s">
@@ -20575,7 +20579,7 @@
       <c r="A18" s="31"/>
       <c r="B18" s="33"/>
       <c r="C18" s="29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="20" t="s">
@@ -20609,7 +20613,7 @@
       <c r="A19" s="31"/>
       <c r="B19" s="33"/>
       <c r="C19" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D19" s="21"/>
       <c r="E19" s="20" t="s">
@@ -20643,7 +20647,7 @@
       <c r="A20" s="31"/>
       <c r="B20" s="33"/>
       <c r="C20" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D20" s="21"/>
       <c r="E20" s="20" t="s">
@@ -20677,7 +20681,7 @@
       <c r="A21" s="31"/>
       <c r="B21" s="33"/>
       <c r="C21" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D21" s="21"/>
       <c r="E21" s="20" t="s">
@@ -20711,7 +20715,7 @@
       <c r="A22" s="31"/>
       <c r="B22" s="33"/>
       <c r="C22" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="20" t="s">
@@ -20745,7 +20749,7 @@
       <c r="A23" s="31"/>
       <c r="B23" s="33"/>
       <c r="C23" s="29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D23" s="21"/>
       <c r="E23" s="20" t="s">
@@ -20776,7 +20780,7 @@
       <c r="A24" s="31"/>
       <c r="B24" s="33"/>
       <c r="C24" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="20" t="s">
@@ -20807,7 +20811,7 @@
       <c r="A25" s="31"/>
       <c r="B25" s="33"/>
       <c r="C25" s="29" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D25" s="21"/>
       <c r="E25" s="20" t="s">
@@ -20838,7 +20842,7 @@
       <c r="A26" s="31"/>
       <c r="B26" s="33"/>
       <c r="C26" s="29" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="20" t="s">
@@ -20900,7 +20904,7 @@
       <c r="A28" s="31"/>
       <c r="B28" s="33"/>
       <c r="C28" s="29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D28" s="21"/>
       <c r="E28" s="20" t="s">
@@ -20962,7 +20966,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="33"/>
       <c r="C30" s="29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D30" s="21"/>
       <c r="E30" s="20" t="s">
@@ -20993,7 +20997,7 @@
       <c r="A31" s="21"/>
       <c r="B31" s="33"/>
       <c r="C31" s="29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="20" t="s">
@@ -21024,7 +21028,7 @@
       <c r="A32" s="21"/>
       <c r="B32" s="33"/>
       <c r="C32" s="29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D32" s="21"/>
       <c r="E32" s="20" t="s">
@@ -21055,7 +21059,7 @@
       <c r="A33" s="21"/>
       <c r="B33" s="33"/>
       <c r="C33" s="29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D33" s="21"/>
       <c r="E33" s="20" t="s">
@@ -21086,7 +21090,7 @@
       <c r="A34" s="21"/>
       <c r="B34" s="33"/>
       <c r="C34" s="29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D34" s="21"/>
       <c r="E34" s="20" t="s">
@@ -21117,7 +21121,7 @@
       <c r="A35" s="21"/>
       <c r="B35" s="33"/>
       <c r="C35" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D35" s="21"/>
       <c r="E35" s="20" t="s">
@@ -21148,7 +21152,7 @@
       <c r="A36" s="21"/>
       <c r="B36" s="33"/>
       <c r="C36" s="29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D36" s="21"/>
       <c r="E36" s="20" t="s">
@@ -21179,7 +21183,7 @@
       <c r="A37" s="21"/>
       <c r="B37" s="33"/>
       <c r="C37" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D37" s="21"/>
       <c r="E37" s="20" t="s">
@@ -21210,7 +21214,7 @@
       <c r="A38" s="21"/>
       <c r="B38" s="33"/>
       <c r="C38" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D38" s="21"/>
       <c r="E38" s="20" t="s">
@@ -21241,7 +21245,7 @@
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="29" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D39" s="21"/>
       <c r="E39" s="20" t="s">
@@ -21272,7 +21276,7 @@
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="20" t="s">

</xml_diff>

<commit_message>
test OF elution buffer
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.17.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.17.balsamic.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="510">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -4809,7 +4809,7 @@
   <dimension ref="A1:AE428"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="O7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0"/>
@@ -5477,7 +5477,9 @@
         <v>502</v>
       </c>
       <c r="V15" s="180"/>
-      <c r="W15" s="198"/>
+      <c r="W15" s="61" t="s">
+        <v>422</v>
+      </c>
       <c r="X15" s="21">
         <v>5</v>
       </c>
@@ -19779,7 +19781,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$103</xm:f>
@@ -19876,6 +19878,12 @@
           </x14:formula1>
           <xm:sqref>W18:W27 W31:W394</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'[1]Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>W15</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
updated orderform fixture 1508 with latest version
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.17.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.17.balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AF98B8-5F69-C649-93FF-99E8DB35245D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F465F522-3099-4443-87EB-D4C51E30DFAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="44260" windowHeight="21760" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="3820" windowWidth="40440" windowHeight="24580" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="description" localSheetId="2">'Drop down lists'!$C$28</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="488">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1779,12 +1779,12 @@
     <t>Tris-HCl (pH 8-8.5)</t>
   </si>
   <si>
+    <t>UDF/Capture Library version</t>
+  </si>
+  <si>
     <t>whole-genome-1</t>
   </si>
   <si>
-    <t>WGSPCFC015</t>
-  </si>
-  <si>
     <t>whole-genome</t>
   </si>
   <si>
@@ -1806,48 +1806,21 @@
     <t>whole-genome-7</t>
   </si>
   <si>
-    <t>whole-genome-8</t>
-  </si>
-  <si>
-    <t>WGSLIFC060</t>
-  </si>
-  <si>
-    <t>whole-genome-9</t>
-  </si>
-  <si>
-    <t>WGSLIFC090</t>
-  </si>
-  <si>
-    <t>whole-genome-10</t>
-  </si>
-  <si>
-    <t>WGTLIFC030</t>
-  </si>
-  <si>
     <t>whole-exome-1</t>
   </si>
   <si>
-    <t>EXOTTTR025</t>
-  </si>
-  <si>
     <t>whole-exome</t>
   </si>
   <si>
     <t>whole-exome-2</t>
   </si>
   <si>
-    <t>EXOTTTR050</t>
-  </si>
-  <si>
     <t>whole-exome-3</t>
   </si>
   <si>
     <t>cancer-capture-panels-1</t>
   </si>
   <si>
-    <t>PANTTTR015</t>
-  </si>
-  <si>
     <t>cancer-capture-panels</t>
   </si>
   <si>
@@ -1860,18 +1833,12 @@
     <t>rna-1</t>
   </si>
   <si>
-    <t>RNAPOAR030</t>
-  </si>
-  <si>
     <t>rna</t>
   </si>
   <si>
     <t>rna-2</t>
   </si>
   <si>
-    <t>RNLPOAR030</t>
-  </si>
-  <si>
     <t>gene-list-test-1</t>
   </si>
   <si>
@@ -1902,91 +1869,22 @@
     <t>gene-list-test-9</t>
   </si>
   <si>
-    <t>gene-list-test-10</t>
-  </si>
-  <si>
-    <t>gene-list-test-11</t>
-  </si>
-  <si>
-    <t>gene-list-test-12</t>
-  </si>
-  <si>
-    <t>gene-list-test-13</t>
-  </si>
-  <si>
-    <t>gene-list-test-14</t>
-  </si>
-  <si>
-    <t>gene-list-test-15</t>
-  </si>
-  <si>
-    <t>gene-list-test-16</t>
-  </si>
-  <si>
-    <t>gene-list-test-17</t>
-  </si>
-  <si>
-    <t>gene-list-test-18</t>
-  </si>
-  <si>
-    <t>gene-list-test-19</t>
-  </si>
-  <si>
-    <t>gene-list-test-20</t>
-  </si>
-  <si>
-    <t>gene-list-test-21</t>
-  </si>
-  <si>
-    <t>gene-list-test-22</t>
-  </si>
-  <si>
-    <t>gene-list-test-23</t>
-  </si>
-  <si>
-    <t>gene-list-test-24</t>
-  </si>
-  <si>
-    <t>gene-list-test-25</t>
-  </si>
-  <si>
-    <t>gene-list-test-26</t>
-  </si>
-  <si>
-    <t>gene-list-test-27</t>
-  </si>
-  <si>
-    <t>gene-list-test-28</t>
-  </si>
-  <si>
-    <t>gene-list-test-29</t>
-  </si>
-  <si>
-    <t>gene-list-test-30</t>
-  </si>
-  <si>
-    <t>gene-list-test-31</t>
-  </si>
-  <si>
-    <t>gene-list-test-32</t>
-  </si>
-  <si>
-    <t>gene-list-test-33</t>
-  </si>
-  <si>
-    <t>gene-list-test-34</t>
-  </si>
-  <si>
     <t>plate</t>
   </si>
   <si>
-    <t>SCN</t>
-  </si>
-  <si>
-    <t>SHANK1</t>
-  </si>
-  <si>
-    <t>SHP</t>
+    <t>LymphoMATIC</t>
+  </si>
+  <si>
+    <t>GIcfDNA</t>
+  </si>
+  <si>
+    <t>GMCKsolid</t>
+  </si>
+  <si>
+    <t>GMSmyeloid</t>
+  </si>
+  <si>
+    <t>other (specify in comment field)</t>
   </si>
   <si>
     <t>1</t>
@@ -1995,28 +1893,64 @@
     <t>comment</t>
   </si>
   <si>
-    <t>LymphoMATIC</t>
-  </si>
-  <si>
-    <t>GIcfDNA</t>
-  </si>
-  <si>
-    <t>GMCKsolid</t>
-  </si>
-  <si>
-    <t>GMSmyeloid</t>
-  </si>
-  <si>
-    <t>other (specify in comment field)</t>
-  </si>
-  <si>
-    <t>Other elution buffer</t>
+    <t>whole-exome-4</t>
+  </si>
+  <si>
+    <t>whole-exome-5</t>
+  </si>
+  <si>
+    <t>whole-exome-6</t>
+  </si>
+  <si>
+    <t>whole-exome-7</t>
+  </si>
+  <si>
+    <t>whole-exome-8</t>
+  </si>
+  <si>
+    <t>whole-exome-9</t>
+  </si>
+  <si>
+    <t>whole-exome-10</t>
+  </si>
+  <si>
+    <t>whole-exome-11</t>
+  </si>
+  <si>
+    <t>whole-exome-12</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-4</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-5</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-6</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-7</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-8</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-9</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-10</t>
+  </si>
+  <si>
+    <t>rna-3</t>
+  </si>
+  <si>
+    <t>rna-4</t>
+  </si>
+  <si>
+    <t>rna-5</t>
   </si>
   <si>
     <t>UDF/Sample Buffer</t>
-  </si>
-  <si>
-    <t>UDF/Capture Library version</t>
   </si>
 </sst>
 </file>
@@ -2629,7 +2563,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="342">
+  <cellStyleXfs count="334">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2967,16 +2901,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="211">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3524,13 +3450,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="47" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -3575,7 +3494,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="342">
+  <cellStyles count="334">
     <cellStyle name="Excel Built-in Normal" xfId="45" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
@@ -3867,14 +3786,6 @@
     <cellStyle name="Följd hyperlänk" xfId="331" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="332" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="333" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="334" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="335" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="336" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="337" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="338" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="339" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="340" builtinId="9" hidden="1"/>
-    <cellStyle name="Följd hyperlänk" xfId="341" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
@@ -4013,7 +3924,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>2310553</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>44874</xdr:rowOff>
+      <xdr:rowOff>217594</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4472,8 +4383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+    <sheetView topLeftCell="A9" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4514,7 +4425,7 @@
         <v>24</v>
       </c>
       <c r="E3" s="170">
-        <v>43593</v>
+        <v>43594</v>
       </c>
     </row>
     <row r="4" spans="1:5" hidden="1">
@@ -4533,8 +4444,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" hidden="1" customHeight="1"/>
-    <row r="6" spans="1:5" ht="14" hidden="1" customHeight="1"/>
-    <row r="7" spans="1:5" ht="1" customHeight="1"/>
+    <row r="6" spans="1:5" ht="1" hidden="1" customHeight="1"/>
+    <row r="7" spans="1:5" ht="1" hidden="1" customHeight="1"/>
+    <row r="8" spans="1:5" hidden="1"/>
     <row r="14" spans="1:5" ht="19">
       <c r="A14" s="40" t="s">
         <v>248</v>
@@ -4806,7 +4718,7 @@
       <c r="A83" s="15"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Ya6vJi5sT7xHyWaAmuube4GzTz15Vio1eC2QkPjfGpjdt5Xyw9+s4tb/NCIfMXkrL4rYJXjRFnHLYWol7oRHTA==" saltValue="7+gFkAOuwcPxd1ACsHf2mw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="9RBRmiHQiWKUjnTrxAAeo604h6ddJA24/1hpreXw4rnwxS1h/CtP1B7pJZMbY5om9yLYzr2p8pO8uQfbpgX3VQ==" saltValue="FYhtGQ/zzJzcwQcnkKcBuA==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -4828,8 +4740,8 @@
   </sheetPr>
   <dimension ref="A1:AE428"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5123,51 +5035,51 @@
       <c r="AE8" s="96"/>
     </row>
     <row r="9" spans="1:31" s="102" customFormat="1" ht="22" customHeight="1" outlineLevel="1">
-      <c r="A9" s="201" t="s">
+      <c r="A9" s="199" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="202"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="202"/>
-      <c r="H9" s="202"/>
-      <c r="I9" s="202"/>
-      <c r="J9" s="202"/>
-      <c r="K9" s="203"/>
+      <c r="B9" s="200"/>
+      <c r="C9" s="200"/>
+      <c r="D9" s="200"/>
+      <c r="E9" s="200"/>
+      <c r="F9" s="200"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="200"/>
+      <c r="I9" s="200"/>
+      <c r="J9" s="200"/>
+      <c r="K9" s="201"/>
       <c r="L9" s="98"/>
-      <c r="M9" s="204" t="s">
+      <c r="M9" s="202" t="s">
         <v>104</v>
       </c>
-      <c r="N9" s="205"/>
+      <c r="N9" s="203"/>
       <c r="O9" s="99"/>
-      <c r="P9" s="207" t="s">
+      <c r="P9" s="205" t="s">
         <v>349</v>
       </c>
-      <c r="Q9" s="208"/>
-      <c r="R9" s="208"/>
-      <c r="S9" s="209"/>
+      <c r="Q9" s="206"/>
+      <c r="R9" s="206"/>
+      <c r="S9" s="207"/>
       <c r="T9" s="100"/>
       <c r="U9" s="183" t="s">
         <v>383</v>
       </c>
       <c r="V9" s="101"/>
-      <c r="W9" s="200" t="s">
+      <c r="W9" s="198" t="s">
         <v>384</v>
       </c>
-      <c r="X9" s="200"/>
+      <c r="X9" s="198"/>
       <c r="Y9" s="101"/>
-      <c r="Z9" s="210" t="s">
+      <c r="Z9" s="208" t="s">
         <v>350</v>
       </c>
-      <c r="AA9" s="211"/>
-      <c r="AB9" s="212"/>
+      <c r="AA9" s="209"/>
+      <c r="AB9" s="210"/>
       <c r="AC9" s="100"/>
-      <c r="AD9" s="206" t="s">
+      <c r="AD9" s="204" t="s">
         <v>205</v>
       </c>
-      <c r="AE9" s="206"/>
+      <c r="AE9" s="204"/>
     </row>
     <row r="10" spans="1:31" s="102" customFormat="1" ht="13" customHeight="1">
       <c r="A10" s="103" t="s">
@@ -5260,11 +5172,11 @@
       </c>
       <c r="T11" s="114"/>
       <c r="U11" s="194" t="s">
-        <v>509</v>
+        <v>430</v>
       </c>
       <c r="V11" s="179"/>
       <c r="W11" s="195" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="X11" s="115" t="s">
         <v>278</v>
@@ -5442,7 +5354,7 @@
     </row>
     <row r="15" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
       <c r="A15" s="55" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B15" s="53" t="s">
         <v>37</v>
@@ -5451,7 +5363,7 @@
         <v>299</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>431</v>
+        <v>285</v>
       </c>
       <c r="E15" s="55" t="s">
         <v>432</v>
@@ -5476,7 +5388,7 @@
       </c>
       <c r="L15" s="149"/>
       <c r="M15" s="58" t="s">
-        <v>496</v>
+        <v>460</v>
       </c>
       <c r="N15" s="57" t="s">
         <v>27</v>
@@ -5491,12 +5403,12 @@
       <c r="R15" s="55" t="s">
         <v>433</v>
       </c>
-      <c r="S15" s="199" t="s">
+      <c r="S15" s="197" t="s">
         <v>434</v>
       </c>
       <c r="T15" s="150"/>
       <c r="U15" s="21" t="s">
-        <v>502</v>
+        <v>461</v>
       </c>
       <c r="V15" s="180"/>
       <c r="W15" s="61" t="s">
@@ -5517,10 +5429,10 @@
       </c>
       <c r="AC15" s="152"/>
       <c r="AD15" s="58" t="s">
-        <v>500</v>
+        <v>466</v>
       </c>
       <c r="AE15" s="58" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:31" s="126" customFormat="1" ht="25" customHeight="1">
@@ -5534,7 +5446,7 @@
         <v>299</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E16" s="55" t="s">
         <v>432</v>
@@ -5571,10 +5483,10 @@
       <c r="S16" s="60"/>
       <c r="T16" s="150"/>
       <c r="U16" s="33" t="s">
-        <v>503</v>
+        <v>462</v>
       </c>
       <c r="V16" s="180"/>
-      <c r="W16" s="198"/>
+      <c r="W16" s="61"/>
       <c r="X16" s="21">
         <v>10</v>
       </c>
@@ -5636,10 +5548,10 @@
       <c r="S17" s="60"/>
       <c r="T17" s="150"/>
       <c r="U17" s="21" t="s">
-        <v>504</v>
+        <v>463</v>
       </c>
       <c r="V17" s="180"/>
-      <c r="W17" s="198"/>
+      <c r="W17" s="61"/>
       <c r="X17" s="21">
         <v>15</v>
       </c>
@@ -5699,7 +5611,7 @@
       <c r="S18" s="60"/>
       <c r="T18" s="150"/>
       <c r="U18" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V18" s="180"/>
       <c r="W18" s="61"/>
@@ -5762,7 +5674,7 @@
       <c r="S19" s="60"/>
       <c r="T19" s="150"/>
       <c r="U19" s="21" t="s">
-        <v>506</v>
+        <v>465</v>
       </c>
       <c r="V19" s="180"/>
       <c r="W19" s="61"/>
@@ -5825,7 +5737,7 @@
       <c r="S20" s="60"/>
       <c r="T20" s="150"/>
       <c r="U20" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V20" s="180"/>
       <c r="W20" s="61"/>
@@ -5851,7 +5763,7 @@
         <v>299</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>290</v>
+        <v>394</v>
       </c>
       <c r="E21" s="55" t="s">
         <v>432</v>
@@ -5888,7 +5800,7 @@
       <c r="S21" s="60"/>
       <c r="T21" s="150"/>
       <c r="U21" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V21" s="180"/>
       <c r="W21" s="61"/>
@@ -5914,10 +5826,10 @@
         <v>299</v>
       </c>
       <c r="D22" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="E22" s="55" t="s">
         <v>440</v>
-      </c>
-      <c r="E22" s="55" t="s">
-        <v>432</v>
       </c>
       <c r="F22" s="54" t="s">
         <v>77</v>
@@ -5951,7 +5863,7 @@
       <c r="S22" s="60"/>
       <c r="T22" s="150"/>
       <c r="U22" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V22" s="180"/>
       <c r="W22" s="61"/>
@@ -5977,10 +5889,10 @@
         <v>299</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>442</v>
+        <v>390</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F23" s="54" t="s">
         <v>77</v>
@@ -6014,7 +5926,7 @@
       <c r="S23" s="60"/>
       <c r="T23" s="150"/>
       <c r="U23" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V23" s="180"/>
       <c r="W23" s="61"/>
@@ -6031,7 +5943,7 @@
     </row>
     <row r="24" spans="1:31" ht="25" customHeight="1">
       <c r="A24" s="55" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B24" s="53" t="s">
         <v>37</v>
@@ -6040,10 +5952,10 @@
         <v>299</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>444</v>
+        <v>391</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="F24" s="54" t="s">
         <v>77</v>
@@ -6077,7 +5989,7 @@
       <c r="S24" s="60"/>
       <c r="T24" s="150"/>
       <c r="U24" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V24" s="180"/>
       <c r="W24" s="61"/>
@@ -6094,7 +6006,7 @@
     </row>
     <row r="25" spans="1:31" ht="25" customHeight="1">
       <c r="A25" s="55" t="s">
-        <v>445</v>
+        <v>468</v>
       </c>
       <c r="B25" s="53" t="s">
         <v>37</v>
@@ -6103,10 +6015,10 @@
         <v>299</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>446</v>
+        <v>392</v>
       </c>
       <c r="E25" s="55" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F25" s="54" t="s">
         <v>77</v>
@@ -6140,7 +6052,7 @@
       <c r="S25" s="60"/>
       <c r="T25" s="150"/>
       <c r="U25" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V25" s="180"/>
       <c r="W25" s="61" t="s">
@@ -6155,13 +6067,11 @@
       <c r="AB25" s="63"/>
       <c r="AC25" s="152"/>
       <c r="AD25" s="58"/>
-      <c r="AE25" s="58" t="s">
-        <v>507</v>
-      </c>
+      <c r="AE25" s="58"/>
     </row>
     <row r="26" spans="1:31" ht="25" customHeight="1">
       <c r="A26" s="55" t="s">
-        <v>448</v>
+        <v>469</v>
       </c>
       <c r="B26" s="53" t="s">
         <v>37</v>
@@ -6170,10 +6080,10 @@
         <v>299</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>449</v>
+        <v>381</v>
       </c>
       <c r="E26" s="55" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>77</v>
@@ -6207,7 +6117,7 @@
       <c r="S26" s="60"/>
       <c r="T26" s="150"/>
       <c r="U26" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V26" s="180"/>
       <c r="W26" s="61" t="s">
@@ -6226,7 +6136,7 @@
     </row>
     <row r="27" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="55" t="s">
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="B27" s="53" t="s">
         <v>37</v>
@@ -6234,11 +6144,11 @@
       <c r="C27" s="54" t="s">
         <v>299</v>
       </c>
-      <c r="D27" s="197" t="s">
-        <v>396</v>
+      <c r="D27" s="29" t="s">
+        <v>395</v>
       </c>
       <c r="E27" s="55" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F27" s="54" t="s">
         <v>77</v>
@@ -6272,7 +6182,7 @@
       <c r="S27" s="60"/>
       <c r="T27" s="150"/>
       <c r="U27" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V27" s="180"/>
       <c r="W27" s="61" t="s">
@@ -6291,7 +6201,7 @@
     </row>
     <row r="28" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="55" t="s">
-        <v>451</v>
+        <v>471</v>
       </c>
       <c r="B28" s="53" t="s">
         <v>37</v>
@@ -6300,10 +6210,10 @@
         <v>299</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>452</v>
+        <v>396</v>
       </c>
       <c r="E28" s="55" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>77</v>
@@ -6337,7 +6247,7 @@
       <c r="S28" s="60"/>
       <c r="T28" s="150"/>
       <c r="U28" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V28" s="180"/>
       <c r="W28" s="61" t="s">
@@ -6356,7 +6266,7 @@
     </row>
     <row r="29" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A29" s="55" t="s">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="B29" s="53" t="s">
         <v>37</v>
@@ -6365,10 +6275,10 @@
         <v>299</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>249</v>
+        <v>397</v>
       </c>
       <c r="E29" s="55" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="F29" s="54" t="s">
         <v>77</v>
@@ -6402,7 +6312,7 @@
       <c r="S29" s="60"/>
       <c r="T29" s="150"/>
       <c r="U29" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V29" s="180"/>
       <c r="W29" s="61" t="s">
@@ -6421,7 +6331,7 @@
     </row>
     <row r="30" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="55" t="s">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="B30" s="53" t="s">
         <v>37</v>
@@ -6430,10 +6340,10 @@
         <v>299</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>364</v>
+        <v>398</v>
       </c>
       <c r="E30" s="55" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="F30" s="54" t="s">
         <v>77</v>
@@ -6467,7 +6377,7 @@
       <c r="S30" s="60"/>
       <c r="T30" s="150"/>
       <c r="U30" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V30" s="180"/>
       <c r="W30" s="61" t="s">
@@ -6486,7 +6396,7 @@
     </row>
     <row r="31" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A31" s="55" t="s">
-        <v>456</v>
+        <v>474</v>
       </c>
       <c r="B31" s="53" t="s">
         <v>37</v>
@@ -6495,10 +6405,10 @@
         <v>299</v>
       </c>
       <c r="D31" s="29" t="s">
-        <v>457</v>
+        <v>399</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>77</v>
@@ -6532,7 +6442,7 @@
       <c r="S31" s="60"/>
       <c r="T31" s="150"/>
       <c r="U31" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V31" s="180"/>
       <c r="W31" s="61"/>
@@ -6549,7 +6459,7 @@
     </row>
     <row r="32" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="55" t="s">
-        <v>459</v>
+        <v>475</v>
       </c>
       <c r="B32" s="53" t="s">
         <v>37</v>
@@ -6558,10 +6468,10 @@
         <v>299</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>460</v>
+        <v>400</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>458</v>
+        <v>440</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>77</v>
@@ -6595,7 +6505,7 @@
       <c r="S32" s="60"/>
       <c r="T32" s="150"/>
       <c r="U32" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V32" s="180"/>
       <c r="W32" s="61"/>
@@ -6611,8 +6521,8 @@
       <c r="AE32" s="58"/>
     </row>
     <row r="33" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
-      <c r="A33" s="39" t="s">
-        <v>461</v>
+      <c r="A33" s="55" t="s">
+        <v>476</v>
       </c>
       <c r="B33" s="53" t="s">
         <v>37</v>
@@ -6621,10 +6531,10 @@
         <v>299</v>
       </c>
       <c r="D33" s="29" t="s">
-        <v>285</v>
+        <v>401</v>
       </c>
       <c r="E33" s="55" t="s">
-        <v>462</v>
+        <v>440</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>77</v>
@@ -6658,7 +6568,7 @@
       <c r="S33" s="60"/>
       <c r="T33" s="150"/>
       <c r="U33" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V33" s="180"/>
       <c r="W33" s="61"/>
@@ -6674,8 +6584,8 @@
       <c r="AE33" s="58"/>
     </row>
     <row r="34" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
-      <c r="A34" s="39" t="s">
-        <v>463</v>
+      <c r="A34" s="55" t="s">
+        <v>443</v>
       </c>
       <c r="B34" s="53" t="s">
         <v>37</v>
@@ -6684,10 +6594,10 @@
         <v>299</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>285</v>
+        <v>406</v>
       </c>
       <c r="E34" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F34" s="54" t="s">
         <v>77</v>
@@ -6721,7 +6631,7 @@
       <c r="S34" s="60"/>
       <c r="T34" s="150"/>
       <c r="U34" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V34" s="180"/>
       <c r="W34" s="61"/>
@@ -6737,8 +6647,8 @@
       <c r="AE34" s="58"/>
     </row>
     <row r="35" spans="1:31" s="153" customFormat="1" ht="25" customHeight="1">
-      <c r="A35" s="39" t="s">
-        <v>464</v>
+      <c r="A35" s="55" t="s">
+        <v>445</v>
       </c>
       <c r="B35" s="53" t="s">
         <v>37</v>
@@ -6747,10 +6657,10 @@
         <v>299</v>
       </c>
       <c r="D35" s="29" t="s">
-        <v>285</v>
+        <v>407</v>
       </c>
       <c r="E35" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>77</v>
@@ -6784,7 +6694,7 @@
       <c r="S35" s="60"/>
       <c r="T35" s="150"/>
       <c r="U35" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V35" s="180"/>
       <c r="W35" s="61"/>
@@ -6800,8 +6710,8 @@
       <c r="AE35" s="58"/>
     </row>
     <row r="36" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
-      <c r="A36" s="39" t="s">
-        <v>465</v>
+      <c r="A36" s="55" t="s">
+        <v>446</v>
       </c>
       <c r="B36" s="53" t="s">
         <v>37</v>
@@ -6810,10 +6720,10 @@
         <v>299</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
       <c r="E36" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>77</v>
@@ -6847,7 +6757,7 @@
       <c r="S36" s="60"/>
       <c r="T36" s="150"/>
       <c r="U36" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V36" s="180"/>
       <c r="W36" s="61"/>
@@ -6863,8 +6773,8 @@
       <c r="AE36" s="58"/>
     </row>
     <row r="37" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
-      <c r="A37" s="39" t="s">
-        <v>466</v>
+      <c r="A37" s="55" t="s">
+        <v>477</v>
       </c>
       <c r="B37" s="53" t="s">
         <v>37</v>
@@ -6873,10 +6783,10 @@
         <v>299</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>285</v>
+        <v>408</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>77</v>
@@ -6910,7 +6820,7 @@
       <c r="S37" s="60"/>
       <c r="T37" s="150"/>
       <c r="U37" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V37" s="180"/>
       <c r="W37" s="61"/>
@@ -6926,8 +6836,8 @@
       <c r="AE37" s="58"/>
     </row>
     <row r="38" spans="1:31" s="154" customFormat="1" ht="25" customHeight="1">
-      <c r="A38" s="39" t="s">
-        <v>467</v>
+      <c r="A38" s="55" t="s">
+        <v>478</v>
       </c>
       <c r="B38" s="53" t="s">
         <v>37</v>
@@ -6936,10 +6846,10 @@
         <v>299</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>285</v>
+        <v>364</v>
       </c>
       <c r="E38" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>77</v>
@@ -6973,7 +6883,7 @@
       <c r="S38" s="60"/>
       <c r="T38" s="150"/>
       <c r="U38" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V38" s="180"/>
       <c r="W38" s="61"/>
@@ -6989,8 +6899,8 @@
       <c r="AE38" s="58"/>
     </row>
     <row r="39" spans="1:31" ht="25" customHeight="1">
-      <c r="A39" s="39" t="s">
-        <v>468</v>
+      <c r="A39" s="55" t="s">
+        <v>479</v>
       </c>
       <c r="B39" s="53" t="s">
         <v>37</v>
@@ -6999,10 +6909,10 @@
         <v>299</v>
       </c>
       <c r="D39" s="29" t="s">
-        <v>285</v>
+        <v>409</v>
       </c>
       <c r="E39" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>77</v>
@@ -7036,7 +6946,7 @@
       <c r="S39" s="60"/>
       <c r="T39" s="150"/>
       <c r="U39" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V39" s="180"/>
       <c r="W39" s="61"/>
@@ -7052,8 +6962,8 @@
       <c r="AE39" s="58"/>
     </row>
     <row r="40" spans="1:31" ht="25" customHeight="1">
-      <c r="A40" s="39" t="s">
-        <v>469</v>
+      <c r="A40" s="55" t="s">
+        <v>480</v>
       </c>
       <c r="B40" s="53" t="s">
         <v>37</v>
@@ -7062,10 +6972,10 @@
         <v>299</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>285</v>
+        <v>410</v>
       </c>
       <c r="E40" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>77</v>
@@ -7099,7 +7009,7 @@
       <c r="S40" s="60"/>
       <c r="T40" s="150"/>
       <c r="U40" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V40" s="180"/>
       <c r="W40" s="61"/>
@@ -7115,8 +7025,8 @@
       <c r="AE40" s="58"/>
     </row>
     <row r="41" spans="1:31" ht="25" customHeight="1">
-      <c r="A41" s="39" t="s">
-        <v>470</v>
+      <c r="A41" s="55" t="s">
+        <v>481</v>
       </c>
       <c r="B41" s="53" t="s">
         <v>37</v>
@@ -7125,10 +7035,10 @@
         <v>299</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>285</v>
+        <v>411</v>
       </c>
       <c r="E41" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>77</v>
@@ -7162,7 +7072,7 @@
       <c r="S41" s="60"/>
       <c r="T41" s="150"/>
       <c r="U41" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V41" s="180"/>
       <c r="W41" s="61"/>
@@ -7178,8 +7088,8 @@
       <c r="AE41" s="58"/>
     </row>
     <row r="42" spans="1:31" ht="25" customHeight="1">
-      <c r="A42" s="39" t="s">
-        <v>471</v>
+      <c r="A42" s="55" t="s">
+        <v>482</v>
       </c>
       <c r="B42" s="53" t="s">
         <v>37</v>
@@ -7188,10 +7098,10 @@
         <v>299</v>
       </c>
       <c r="D42" s="29" t="s">
-        <v>285</v>
+        <v>412</v>
       </c>
       <c r="E42" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>77</v>
@@ -7225,7 +7135,7 @@
       <c r="S42" s="60"/>
       <c r="T42" s="150"/>
       <c r="U42" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V42" s="180"/>
       <c r="W42" s="61"/>
@@ -7241,8 +7151,8 @@
       <c r="AE42" s="58"/>
     </row>
     <row r="43" spans="1:31" ht="25" customHeight="1">
-      <c r="A43" s="39" t="s">
-        <v>472</v>
+      <c r="A43" s="55" t="s">
+        <v>483</v>
       </c>
       <c r="B43" s="53" t="s">
         <v>37</v>
@@ -7251,10 +7161,10 @@
         <v>299</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>285</v>
+        <v>413</v>
       </c>
       <c r="E43" s="55" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>77</v>
@@ -7288,7 +7198,7 @@
       <c r="S43" s="60"/>
       <c r="T43" s="150"/>
       <c r="U43" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V43" s="180"/>
       <c r="W43" s="61"/>
@@ -7304,8 +7214,8 @@
       <c r="AE43" s="58"/>
     </row>
     <row r="44" spans="1:31" ht="25" customHeight="1">
-      <c r="A44" s="39" t="s">
-        <v>473</v>
+      <c r="A44" s="55" t="s">
+        <v>447</v>
       </c>
       <c r="B44" s="53" t="s">
         <v>37</v>
@@ -7314,10 +7224,10 @@
         <v>299</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>285</v>
+        <v>414</v>
       </c>
       <c r="E44" s="55" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>77</v>
@@ -7351,7 +7261,7 @@
       <c r="S44" s="60"/>
       <c r="T44" s="150"/>
       <c r="U44" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V44" s="180"/>
       <c r="W44" s="61"/>
@@ -7367,8 +7277,8 @@
       <c r="AE44" s="58"/>
     </row>
     <row r="45" spans="1:31" ht="25" customHeight="1">
-      <c r="A45" s="39" t="s">
-        <v>474</v>
+      <c r="A45" s="55" t="s">
+        <v>449</v>
       </c>
       <c r="B45" s="53" t="s">
         <v>37</v>
@@ -7377,10 +7287,10 @@
         <v>299</v>
       </c>
       <c r="D45" s="29" t="s">
-        <v>285</v>
+        <v>415</v>
       </c>
       <c r="E45" s="55" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>77</v>
@@ -7414,7 +7324,7 @@
       <c r="S45" s="60"/>
       <c r="T45" s="150"/>
       <c r="U45" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V45" s="180"/>
       <c r="W45" s="61"/>
@@ -7430,8 +7340,8 @@
       <c r="AE45" s="58"/>
     </row>
     <row r="46" spans="1:31" ht="25" customHeight="1">
-      <c r="A46" s="39" t="s">
-        <v>475</v>
+      <c r="A46" s="55" t="s">
+        <v>484</v>
       </c>
       <c r="B46" s="53" t="s">
         <v>37</v>
@@ -7440,10 +7350,10 @@
         <v>299</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>285</v>
+        <v>416</v>
       </c>
       <c r="E46" s="55" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>77</v>
@@ -7477,7 +7387,7 @@
       <c r="S46" s="60"/>
       <c r="T46" s="150"/>
       <c r="U46" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V46" s="180"/>
       <c r="W46" s="61"/>
@@ -7493,8 +7403,8 @@
       <c r="AE46" s="58"/>
     </row>
     <row r="47" spans="1:31" ht="25" customHeight="1">
-      <c r="A47" s="39" t="s">
-        <v>476</v>
+      <c r="A47" s="55" t="s">
+        <v>485</v>
       </c>
       <c r="B47" s="53" t="s">
         <v>37</v>
@@ -7503,10 +7413,10 @@
         <v>299</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>285</v>
+        <v>417</v>
       </c>
       <c r="E47" s="55" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>77</v>
@@ -7540,7 +7450,7 @@
       <c r="S47" s="60"/>
       <c r="T47" s="150"/>
       <c r="U47" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V47" s="180"/>
       <c r="W47" s="61"/>
@@ -7556,8 +7466,8 @@
       <c r="AE47" s="58"/>
     </row>
     <row r="48" spans="1:31" ht="25" customHeight="1">
-      <c r="A48" s="39" t="s">
-        <v>477</v>
+      <c r="A48" s="55" t="s">
+        <v>486</v>
       </c>
       <c r="B48" s="53" t="s">
         <v>37</v>
@@ -7566,10 +7476,10 @@
         <v>299</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>285</v>
+        <v>418</v>
       </c>
       <c r="E48" s="55" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>77</v>
@@ -7603,7 +7513,7 @@
       <c r="S48" s="60"/>
       <c r="T48" s="150"/>
       <c r="U48" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V48" s="180"/>
       <c r="W48" s="61"/>
@@ -7620,7 +7530,7 @@
     </row>
     <row r="49" spans="1:31" ht="25" customHeight="1">
       <c r="A49" s="39" t="s">
-        <v>478</v>
+        <v>450</v>
       </c>
       <c r="B49" s="53" t="s">
         <v>37</v>
@@ -7632,7 +7542,7 @@
         <v>285</v>
       </c>
       <c r="E49" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>77</v>
@@ -7666,7 +7576,7 @@
       <c r="S49" s="60"/>
       <c r="T49" s="150"/>
       <c r="U49" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V49" s="180"/>
       <c r="W49" s="61"/>
@@ -7683,7 +7593,7 @@
     </row>
     <row r="50" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A50" s="39" t="s">
-        <v>479</v>
+        <v>452</v>
       </c>
       <c r="B50" s="53" t="s">
         <v>37</v>
@@ -7695,7 +7605,7 @@
         <v>285</v>
       </c>
       <c r="E50" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>77</v>
@@ -7729,7 +7639,7 @@
       <c r="S50" s="60"/>
       <c r="T50" s="150"/>
       <c r="U50" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V50" s="180"/>
       <c r="W50" s="61"/>
@@ -7746,7 +7656,7 @@
     </row>
     <row r="51" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A51" s="39" t="s">
-        <v>480</v>
+        <v>453</v>
       </c>
       <c r="B51" s="53" t="s">
         <v>37</v>
@@ -7758,7 +7668,7 @@
         <v>285</v>
       </c>
       <c r="E51" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>77</v>
@@ -7792,7 +7702,7 @@
       <c r="S51" s="60"/>
       <c r="T51" s="150"/>
       <c r="U51" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V51" s="180"/>
       <c r="W51" s="61"/>
@@ -7809,7 +7719,7 @@
     </row>
     <row r="52" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A52" s="39" t="s">
-        <v>481</v>
+        <v>454</v>
       </c>
       <c r="B52" s="53" t="s">
         <v>37</v>
@@ -7821,7 +7731,7 @@
         <v>285</v>
       </c>
       <c r="E52" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>77</v>
@@ -7855,7 +7765,7 @@
       <c r="S52" s="60"/>
       <c r="T52" s="150"/>
       <c r="U52" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V52" s="180"/>
       <c r="W52" s="61"/>
@@ -7872,7 +7782,7 @@
     </row>
     <row r="53" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A53" s="39" t="s">
-        <v>482</v>
+        <v>455</v>
       </c>
       <c r="B53" s="53" t="s">
         <v>37</v>
@@ -7884,7 +7794,7 @@
         <v>285</v>
       </c>
       <c r="E53" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>77</v>
@@ -7918,7 +7828,7 @@
       <c r="S53" s="60"/>
       <c r="T53" s="150"/>
       <c r="U53" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V53" s="180"/>
       <c r="W53" s="61"/>
@@ -7935,7 +7845,7 @@
     </row>
     <row r="54" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A54" s="39" t="s">
-        <v>483</v>
+        <v>456</v>
       </c>
       <c r="B54" s="53" t="s">
         <v>37</v>
@@ -7947,7 +7857,7 @@
         <v>285</v>
       </c>
       <c r="E54" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>77</v>
@@ -7981,7 +7891,7 @@
       <c r="S54" s="60"/>
       <c r="T54" s="150"/>
       <c r="U54" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V54" s="180"/>
       <c r="W54" s="61"/>
@@ -7998,7 +7908,7 @@
     </row>
     <row r="55" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A55" s="39" t="s">
-        <v>484</v>
+        <v>457</v>
       </c>
       <c r="B55" s="53" t="s">
         <v>37</v>
@@ -8010,7 +7920,7 @@
         <v>285</v>
       </c>
       <c r="E55" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>77</v>
@@ -8044,7 +7954,7 @@
       <c r="S55" s="60"/>
       <c r="T55" s="150"/>
       <c r="U55" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V55" s="180"/>
       <c r="W55" s="61"/>
@@ -8061,7 +7971,7 @@
     </row>
     <row r="56" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A56" s="39" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="B56" s="53" t="s">
         <v>37</v>
@@ -8073,7 +7983,7 @@
         <v>285</v>
       </c>
       <c r="E56" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>77</v>
@@ -8107,7 +8017,7 @@
       <c r="S56" s="60"/>
       <c r="T56" s="150"/>
       <c r="U56" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V56" s="180"/>
       <c r="W56" s="61"/>
@@ -8124,7 +8034,7 @@
     </row>
     <row r="57" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
       <c r="A57" s="39" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="B57" s="53" t="s">
         <v>37</v>
@@ -8136,7 +8046,7 @@
         <v>285</v>
       </c>
       <c r="E57" s="55" t="s">
-        <v>462</v>
+        <v>451</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>77</v>
@@ -8170,7 +8080,7 @@
       <c r="S57" s="60"/>
       <c r="T57" s="150"/>
       <c r="U57" s="21" t="s">
-        <v>505</v>
+        <v>464</v>
       </c>
       <c r="V57" s="180"/>
       <c r="W57" s="61"/>
@@ -8186,60 +8096,30 @@
       <c r="AE57" s="58"/>
     </row>
     <row r="58" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A58" s="39" t="s">
-        <v>487</v>
-      </c>
-      <c r="B58" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C58" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D58" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E58" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F58" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G58" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H58" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I58" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J58" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K58" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A58" s="39"/>
+      <c r="B58" s="53"/>
+      <c r="C58" s="54"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="56"/>
+      <c r="H58" s="196"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="53"/>
+      <c r="K58" s="28"/>
       <c r="L58" s="149"/>
       <c r="M58" s="58"/>
       <c r="N58" s="57"/>
       <c r="O58" s="149"/>
-      <c r="P58" s="30" t="s">
-        <v>326</v>
-      </c>
-      <c r="Q58" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P58" s="64"/>
+      <c r="Q58" s="56"/>
       <c r="R58" s="59"/>
       <c r="S58" s="60"/>
       <c r="T58" s="150"/>
-      <c r="U58" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U58" s="21"/>
       <c r="V58" s="180"/>
       <c r="W58" s="61"/>
-      <c r="X58" s="21">
-        <v>100</v>
-      </c>
+      <c r="X58" s="21"/>
       <c r="Y58" s="151"/>
       <c r="Z58" s="62"/>
       <c r="AA58" s="62"/>
@@ -8249,60 +8129,30 @@
       <c r="AE58" s="58"/>
     </row>
     <row r="59" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A59" s="39" t="s">
-        <v>488</v>
-      </c>
-      <c r="B59" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D59" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E59" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F59" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G59" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H59" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I59" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J59" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K59" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A59" s="39"/>
+      <c r="B59" s="53"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="54"/>
+      <c r="G59" s="56"/>
+      <c r="H59" s="196"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="53"/>
+      <c r="K59" s="28"/>
       <c r="L59" s="149"/>
       <c r="M59" s="58"/>
       <c r="N59" s="57"/>
       <c r="O59" s="149"/>
-      <c r="P59" s="30" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q59" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P59" s="64"/>
+      <c r="Q59" s="56"/>
       <c r="R59" s="59"/>
       <c r="S59" s="60"/>
       <c r="T59" s="150"/>
-      <c r="U59" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U59" s="21"/>
       <c r="V59" s="180"/>
       <c r="W59" s="61"/>
-      <c r="X59" s="21">
-        <v>100</v>
-      </c>
+      <c r="X59" s="21"/>
       <c r="Y59" s="151"/>
       <c r="Z59" s="62"/>
       <c r="AA59" s="62"/>
@@ -8312,60 +8162,30 @@
       <c r="AE59" s="58"/>
     </row>
     <row r="60" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A60" s="39" t="s">
-        <v>489</v>
-      </c>
-      <c r="B60" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C60" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D60" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E60" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F60" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G60" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H60" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I60" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J60" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K60" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A60" s="39"/>
+      <c r="B60" s="53"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="56"/>
+      <c r="H60" s="196"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="28"/>
       <c r="L60" s="149"/>
       <c r="M60" s="58"/>
       <c r="N60" s="57"/>
       <c r="O60" s="149"/>
-      <c r="P60" s="30" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q60" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P60" s="64"/>
+      <c r="Q60" s="56"/>
       <c r="R60" s="59"/>
       <c r="S60" s="60"/>
       <c r="T60" s="150"/>
-      <c r="U60" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U60" s="21"/>
       <c r="V60" s="180"/>
       <c r="W60" s="61"/>
-      <c r="X60" s="21">
-        <v>100</v>
-      </c>
+      <c r="X60" s="21"/>
       <c r="Y60" s="151"/>
       <c r="Z60" s="62"/>
       <c r="AA60" s="62"/>
@@ -8375,60 +8195,30 @@
       <c r="AE60" s="58"/>
     </row>
     <row r="61" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A61" s="39" t="s">
-        <v>490</v>
-      </c>
-      <c r="B61" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E61" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F61" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G61" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H61" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I61" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J61" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K61" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A61" s="39"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="54"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="56"/>
+      <c r="H61" s="196"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="53"/>
+      <c r="K61" s="28"/>
       <c r="L61" s="149"/>
       <c r="M61" s="58"/>
       <c r="N61" s="57"/>
       <c r="O61" s="149"/>
-      <c r="P61" s="30" t="s">
-        <v>314</v>
-      </c>
-      <c r="Q61" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P61" s="64"/>
+      <c r="Q61" s="56"/>
       <c r="R61" s="59"/>
       <c r="S61" s="60"/>
       <c r="T61" s="150"/>
-      <c r="U61" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U61" s="21"/>
       <c r="V61" s="180"/>
       <c r="W61" s="61"/>
-      <c r="X61" s="21">
-        <v>100</v>
-      </c>
+      <c r="X61" s="21"/>
       <c r="Y61" s="151"/>
       <c r="Z61" s="62"/>
       <c r="AA61" s="62"/>
@@ -8438,60 +8228,30 @@
       <c r="AE61" s="58"/>
     </row>
     <row r="62" spans="1:31" s="155" customFormat="1" ht="25" customHeight="1">
-      <c r="A62" s="39" t="s">
-        <v>491</v>
-      </c>
-      <c r="B62" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D62" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E62" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F62" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G62" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H62" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I62" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J62" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K62" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A62" s="39"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="54"/>
+      <c r="G62" s="56"/>
+      <c r="H62" s="196"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="53"/>
+      <c r="K62" s="28"/>
       <c r="L62" s="149"/>
       <c r="M62" s="58"/>
       <c r="N62" s="57"/>
       <c r="O62" s="149"/>
-      <c r="P62" s="30" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q62" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P62" s="64"/>
+      <c r="Q62" s="56"/>
       <c r="R62" s="59"/>
       <c r="S62" s="60"/>
       <c r="T62" s="150"/>
-      <c r="U62" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U62" s="21"/>
       <c r="V62" s="180"/>
       <c r="W62" s="61"/>
-      <c r="X62" s="21">
-        <v>100</v>
-      </c>
+      <c r="X62" s="21"/>
       <c r="Y62" s="151"/>
       <c r="Z62" s="62"/>
       <c r="AA62" s="62"/>
@@ -8501,60 +8261,30 @@
       <c r="AE62" s="58"/>
     </row>
     <row r="63" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
-      <c r="A63" s="39" t="s">
-        <v>492</v>
-      </c>
-      <c r="B63" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E63" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F63" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G63" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H63" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I63" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J63" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K63" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A63" s="39"/>
+      <c r="B63" s="53"/>
+      <c r="C63" s="54"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="54"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="196"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="53"/>
+      <c r="K63" s="28"/>
       <c r="L63" s="149"/>
       <c r="M63" s="58"/>
       <c r="N63" s="57"/>
       <c r="O63" s="149"/>
-      <c r="P63" s="166" t="s">
-        <v>498</v>
-      </c>
-      <c r="Q63" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P63" s="64"/>
+      <c r="Q63" s="56"/>
       <c r="R63" s="59"/>
       <c r="S63" s="60"/>
       <c r="T63" s="150"/>
-      <c r="U63" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U63" s="21"/>
       <c r="V63" s="180"/>
       <c r="W63" s="61"/>
-      <c r="X63" s="21">
-        <v>100</v>
-      </c>
+      <c r="X63" s="21"/>
       <c r="Y63" s="151"/>
       <c r="Z63" s="62"/>
       <c r="AA63" s="62"/>
@@ -8564,60 +8294,30 @@
       <c r="AE63" s="58"/>
     </row>
     <row r="64" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
-      <c r="A64" s="39" t="s">
-        <v>493</v>
-      </c>
-      <c r="B64" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C64" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E64" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F64" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G64" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H64" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I64" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J64" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K64" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A64" s="39"/>
+      <c r="B64" s="53"/>
+      <c r="C64" s="54"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="56"/>
+      <c r="H64" s="196"/>
+      <c r="I64" s="20"/>
+      <c r="J64" s="53"/>
+      <c r="K64" s="28"/>
       <c r="L64" s="149"/>
       <c r="M64" s="58"/>
       <c r="N64" s="57"/>
       <c r="O64" s="149"/>
-      <c r="P64" s="166" t="s">
-        <v>499</v>
-      </c>
-      <c r="Q64" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P64" s="64"/>
+      <c r="Q64" s="56"/>
       <c r="R64" s="59"/>
       <c r="S64" s="60"/>
       <c r="T64" s="150"/>
-      <c r="U64" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U64" s="21"/>
       <c r="V64" s="180"/>
       <c r="W64" s="61"/>
-      <c r="X64" s="21">
-        <v>100</v>
-      </c>
+      <c r="X64" s="21"/>
       <c r="Y64" s="151"/>
       <c r="Z64" s="62"/>
       <c r="AA64" s="62"/>
@@ -8627,60 +8327,30 @@
       <c r="AE64" s="58"/>
     </row>
     <row r="65" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
-      <c r="A65" s="39" t="s">
-        <v>494</v>
-      </c>
-      <c r="B65" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C65" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D65" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E65" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F65" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G65" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H65" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I65" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J65" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K65" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A65" s="39"/>
+      <c r="B65" s="53"/>
+      <c r="C65" s="54"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="54"/>
+      <c r="G65" s="56"/>
+      <c r="H65" s="196"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="53"/>
+      <c r="K65" s="28"/>
       <c r="L65" s="149"/>
       <c r="M65" s="58"/>
       <c r="N65" s="57"/>
       <c r="O65" s="149"/>
-      <c r="P65" s="166" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q65" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P65" s="64"/>
+      <c r="Q65" s="56"/>
       <c r="R65" s="59"/>
       <c r="S65" s="60"/>
       <c r="T65" s="150"/>
-      <c r="U65" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U65" s="21"/>
       <c r="V65" s="180"/>
       <c r="W65" s="61"/>
-      <c r="X65" s="21">
-        <v>100</v>
-      </c>
+      <c r="X65" s="21"/>
       <c r="Y65" s="151"/>
       <c r="Z65" s="62"/>
       <c r="AA65" s="62"/>
@@ -8690,60 +8360,30 @@
       <c r="AE65" s="58"/>
     </row>
     <row r="66" spans="1:31" s="156" customFormat="1" ht="25" customHeight="1">
-      <c r="A66" s="39" t="s">
-        <v>495</v>
-      </c>
-      <c r="B66" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="C66" s="54" t="s">
-        <v>299</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="E66" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="F66" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="G66" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="H66" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="I66" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="J66" s="53" t="s">
-        <v>93</v>
-      </c>
-      <c r="K66" s="28" t="s">
-        <v>17</v>
-      </c>
+      <c r="A66" s="39"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="54"/>
+      <c r="G66" s="56"/>
+      <c r="H66" s="196"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="53"/>
+      <c r="K66" s="28"/>
       <c r="L66" s="149"/>
       <c r="M66" s="58"/>
       <c r="N66" s="57"/>
       <c r="O66" s="149"/>
-      <c r="P66" s="166" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q66" s="56" t="s">
-        <v>77</v>
-      </c>
+      <c r="P66" s="64"/>
+      <c r="Q66" s="56"/>
       <c r="R66" s="59"/>
       <c r="S66" s="60"/>
       <c r="T66" s="150"/>
-      <c r="U66" s="21" t="s">
-        <v>505</v>
-      </c>
+      <c r="U66" s="21"/>
       <c r="V66" s="180"/>
       <c r="W66" s="61"/>
-      <c r="X66" s="21">
-        <v>100</v>
-      </c>
+      <c r="X66" s="21"/>
       <c r="Y66" s="151"/>
       <c r="Z66" s="62"/>
       <c r="AA66" s="62"/>
@@ -19828,77 +19468,77 @@
           </x14:formula1>
           <xm:sqref>K15:K394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$H$3:$H$4</xm:f>
           </x14:formula1>
           <xm:sqref>G15:G394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$J$3:$J$5</xm:f>
           </x14:formula1>
           <xm:sqref>Q15:Q394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$B$3:$B$6</xm:f>
           </x14:formula1>
           <xm:sqref>C15:C394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$I$3:$I$7</xm:f>
           </x14:formula1>
           <xm:sqref>I15:I394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$O$3:$O$4</xm:f>
           </x14:formula1>
           <xm:sqref>AB15:AB394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000A000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$F$3:$F$4</xm:f>
           </x14:formula1>
           <xm:sqref>G15:G394 J15:K394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000B000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E8BB804-807E-CA4C-93E7-0832B67F3EC1}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$N$3:$N$22</xm:f>
           </x14:formula1>
           <xm:sqref>X15:X394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000C000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$G$3:$G$14</xm:f>
           </x14:formula1>
           <xm:sqref>K15:K394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{721A107B-6D1D-5F41-B605-61665D3A323C}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$G$3:$G$15</xm:f>
           </x14:formula1>
           <xm:sqref>H15:H394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{00000000-0002-0000-0100-00000E000000}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$C$3:$C$40</xm:f>
-          </x14:formula1>
-          <xm:sqref>D15:D394</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000F000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$M$3:$M$45</xm:f>
           </x14:formula1>
           <xm:sqref>P15:P394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000010000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3DB8F3B2-ED07-314E-8B12-E986A210F9E2}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$K$3:$K$5</xm:f>
           </x14:formula1>
-          <xm:sqref>W18:W27 W31:W394 W15</xm:sqref>
+          <xm:sqref>W15:W394</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{4B818C0C-591E-D74F-998D-F811DA860665}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!$C$3:$C$40</xm:f>
+          </x14:formula1>
+          <xm:sqref>D15:D63 D67:D394</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -19914,7 +19554,7 @@
   <dimension ref="A1:AL103"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M45"/>
+      <selection activeCell="C40" sqref="C4:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
add skin as a source
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.17.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.17.balsamic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F465F522-3099-4443-87EB-D4C51E30DFAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D077752F-3D14-2044-97F2-7630085D9C6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="3820" windowWidth="40440" windowHeight="24580" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4315,7 +4315,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4359,7 +4359,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4741,7 +4741,7 @@
   <dimension ref="A1:AE428"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5649,7 +5649,7 @@
         <v>93</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>377</v>
+        <v>252</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>102</v>
@@ -5711,8 +5711,8 @@
       <c r="G20" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="20" t="s">
-        <v>98</v>
+      <c r="H20" s="173" t="s">
+        <v>377</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>102</v>
@@ -5774,8 +5774,8 @@
       <c r="G21" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="20" t="s">
-        <v>99</v>
+      <c r="H21" s="173" t="s">
+        <v>387</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>102</v>
@@ -5838,7 +5838,7 @@
         <v>93</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>246</v>
+        <v>98</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>102</v>
@@ -5900,8 +5900,8 @@
       <c r="G23" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="41" t="s">
-        <v>252</v>
+      <c r="H23" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>102</v>
@@ -5963,8 +5963,8 @@
       <c r="G24" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="196" t="s">
-        <v>356</v>
+      <c r="H24" s="20" t="s">
+        <v>246</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>102</v>
@@ -6027,7 +6027,7 @@
         <v>93</v>
       </c>
       <c r="H25" s="196" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>102</v>
@@ -6091,8 +6091,8 @@
       <c r="G26" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="20" t="s">
-        <v>100</v>
+      <c r="H26" s="196" t="s">
+        <v>357</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>102</v>
@@ -6156,8 +6156,8 @@
       <c r="G27" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H27" s="196" t="s">
-        <v>357</v>
+      <c r="H27" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="I27" s="20" t="s">
         <v>102</v>
@@ -19443,7 +19443,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$103</xm:f>
@@ -19520,7 +19520,7 @@
           <x14:formula1>
             <xm:f>'Drop down lists'!$G$3:$G$15</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:H394</xm:sqref>
+          <xm:sqref>H28:H394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
@@ -19539,6 +19539,12 @@
             <xm:f>'Drop down lists'!$C$3:$C$40</xm:f>
           </x14:formula1>
           <xm:sqref>D15:D63 D67:D394</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AC34195-0310-EA42-A915-67A0B3B7E950}">
+          <x14:formula1>
+            <xm:f>'[1508.17.fastq.xlsx]Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>H15:H27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
feat(UI): add skin as a source in the order portal (#382)
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.17.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.17.balsamic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F465F522-3099-4443-87EB-D4C51E30DFAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D077752F-3D14-2044-97F2-7630085D9C6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="3820" windowWidth="40440" windowHeight="24580" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4315,7 +4315,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4359,7 +4359,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4741,7 +4741,7 @@
   <dimension ref="A1:AE428"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -5649,7 +5649,7 @@
         <v>93</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>377</v>
+        <v>252</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>102</v>
@@ -5711,8 +5711,8 @@
       <c r="G20" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="20" t="s">
-        <v>98</v>
+      <c r="H20" s="173" t="s">
+        <v>377</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>102</v>
@@ -5774,8 +5774,8 @@
       <c r="G21" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H21" s="20" t="s">
-        <v>99</v>
+      <c r="H21" s="173" t="s">
+        <v>387</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>102</v>
@@ -5838,7 +5838,7 @@
         <v>93</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>246</v>
+        <v>98</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>102</v>
@@ -5900,8 +5900,8 @@
       <c r="G23" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H23" s="41" t="s">
-        <v>252</v>
+      <c r="H23" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="I23" s="20" t="s">
         <v>102</v>
@@ -5963,8 +5963,8 @@
       <c r="G24" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="196" t="s">
-        <v>356</v>
+      <c r="H24" s="20" t="s">
+        <v>246</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>102</v>
@@ -6027,7 +6027,7 @@
         <v>93</v>
       </c>
       <c r="H25" s="196" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>102</v>
@@ -6091,8 +6091,8 @@
       <c r="G26" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="20" t="s">
-        <v>100</v>
+      <c r="H26" s="196" t="s">
+        <v>357</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>102</v>
@@ -6156,8 +6156,8 @@
       <c r="G27" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="H27" s="196" t="s">
-        <v>357</v>
+      <c r="H27" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="I27" s="20" t="s">
         <v>102</v>
@@ -19443,7 +19443,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="17">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$103</xm:f>
@@ -19520,7 +19520,7 @@
           <x14:formula1>
             <xm:f>'Drop down lists'!$G$3:$G$15</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:H394</xm:sqref>
+          <xm:sqref>H28:H394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-00000D000000}">
           <x14:formula1>
@@ -19539,6 +19539,12 @@
             <xm:f>'Drop down lists'!$C$3:$C$40</xm:f>
           </x14:formula1>
           <xm:sqref>D15:D63 D67:D394</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3AC34195-0310-EA42-A915-67A0B3B7E950}">
+          <x14:formula1>
+            <xm:f>'[1508.17.fastq.xlsx]Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>H15:H27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>